<commit_message>
pemisah ribuan dengan koma saja. menuju CRUD
</commit_message>
<xml_diff>
--- a/data/monalisa_sjb.xlsx
+++ b/data/monalisa_sjb.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18750" windowHeight="6800"/>
+    <workbookView windowWidth="18750" windowHeight="6800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="kinerja_bulanan" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="22">
   <si>
     <t>kpknl</t>
   </si>
@@ -69,6 +69,9 @@
     <t>KPKNL Pangkal Pinang</t>
   </si>
   <si>
+    <t>Pejabat Lelang Kelas II</t>
+  </si>
+  <si>
     <t>pokok_q1</t>
   </si>
   <si>
@@ -91,25 +94,19 @@
   </si>
   <si>
     <t>pnbp_q4</t>
-  </si>
-  <si>
-    <t>Pejabat Lelang Kelas II</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="7">
+  <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,13 +117,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -275,11 +265,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -597,163 +582,160 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -803,8 +785,6 @@
     <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
-    <cellStyle name="Comma 2" xfId="49"/>
-    <cellStyle name="Comma 2 3" xfId="50"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1107,18 +1087,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="20.6363636363636" customWidth="1"/>
-    <col min="6" max="6" width="18.3636363636364"/>
-    <col min="7" max="7" width="17.1818181818182"/>
-    <col min="8" max="9" width="15.5454545454545"/>
+    <col min="6" max="6" width="12.8181818181818"/>
+    <col min="7" max="7" width="11.7272727272727"/>
+    <col min="8" max="9" width="10.5454545454545"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1150,7 +1129,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1166,17 +1145,14 @@
       <c r="E2">
         <v>187</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2">
         <v>28436387900</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2">
         <v>1048182978</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2">
         <v>567411775</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1195,16 +1171,16 @@
       <c r="E3">
         <v>131</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3">
         <v>8774078570</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3">
         <v>260932373</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3">
         <v>64840375</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3">
         <v>918481182</v>
       </c>
     </row>
@@ -1224,16 +1200,16 @@
       <c r="E4">
         <v>279</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4">
         <v>22744381408</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4">
         <v>687374956</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4">
         <v>222773463</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4">
         <v>115191249</v>
       </c>
     </row>
@@ -1253,16 +1229,16 @@
       <c r="E5">
         <v>191</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5">
         <v>15850619013</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5">
         <v>489872355</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5">
         <v>193480693</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5">
         <v>164303200</v>
       </c>
     </row>
@@ -1282,16 +1258,16 @@
       <c r="E6">
         <v>168</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6">
         <v>9284728199</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6">
         <v>295239561</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6">
         <v>96138250</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6">
         <v>106771995</v>
       </c>
     </row>
@@ -1311,16 +1287,16 @@
       <c r="E7">
         <v>99</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7">
         <v>20471496109</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7">
         <v>922321034</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7">
         <v>367583115</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7">
         <v>697666230</v>
       </c>
     </row>
@@ -1340,16 +1316,16 @@
       <c r="E8">
         <v>115</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8">
         <v>13782029501</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8">
         <v>435251854</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8">
         <v>86296257.5</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8">
         <v>122230565</v>
       </c>
     </row>
@@ -1369,16 +1345,16 @@
       <c r="E9">
         <v>126</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9">
         <v>18793350488</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9">
         <v>522735209</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9">
         <v>111960250</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9">
         <v>167920500</v>
       </c>
     </row>
@@ -1398,16 +1374,16 @@
       <c r="E10">
         <v>123</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10">
         <v>15757602878</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10">
         <v>572865367</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10">
         <v>281172510</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10">
         <v>498345020</v>
       </c>
     </row>
@@ -1427,20 +1403,20 @@
       <c r="E11">
         <v>168</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11">
         <v>23397422689</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11">
         <v>751880985</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11">
         <v>276898575</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11">
         <v>461767150</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1456,20 +1432,17 @@
       <c r="E12">
         <v>24</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12">
         <v>172604700</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12">
         <v>9952094</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12">
         <v>3250000</v>
       </c>
-      <c r="I12" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1485,17 +1458,14 @@
       <c r="E13">
         <v>85</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13">
         <v>2978835200</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13">
         <v>79557704</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13">
         <v>13413750</v>
-      </c>
-      <c r="I13" s="2">
-        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1514,16 +1484,16 @@
       <c r="E14">
         <v>141</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14">
         <v>7323407755</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14">
         <v>206085656</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14">
         <v>28592500</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14">
         <v>11325000</v>
       </c>
     </row>
@@ -1543,20 +1513,20 @@
       <c r="E15">
         <v>57</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15">
         <v>1903857200</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15">
         <v>63416144</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15">
         <v>19305000</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15">
         <v>10280000</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1572,20 +1542,17 @@
       <c r="E16">
         <v>69</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16">
         <v>5876359800</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16">
         <v>197278956</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16">
         <v>8837500</v>
       </c>
-      <c r="I16" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1601,17 +1568,14 @@
       <c r="E17">
         <v>63</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17">
         <v>1489350200</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17">
         <v>55620044</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17">
         <v>10050000</v>
-      </c>
-      <c r="I17" s="2">
-        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1630,16 +1594,16 @@
       <c r="E18">
         <v>139</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18">
         <v>5758998700</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18">
         <v>197369304</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18">
         <v>78662650</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18">
         <v>33710850</v>
       </c>
     </row>
@@ -1659,16 +1623,16 @@
       <c r="E19">
         <v>147</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19">
         <v>6058766000</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19">
         <v>155608500</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19">
         <v>21938975</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19">
         <v>124089550</v>
       </c>
     </row>
@@ -1688,16 +1652,16 @@
       <c r="E20">
         <v>156</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20">
         <v>1850945676</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20">
         <v>68543557</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20">
         <v>34532500</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20">
         <v>587200</v>
       </c>
     </row>
@@ -1717,17 +1681,132 @@
       <c r="E21">
         <v>127</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21">
         <v>8549514067</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21">
         <v>266064627</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21">
         <v>34675000</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I21">
         <v>20172150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22">
+        <v>2025</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>25</v>
+      </c>
+      <c r="F22">
+        <v>84597380000</v>
+      </c>
+      <c r="G22">
+        <v>507584280</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23">
+        <v>2025</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>29</v>
+      </c>
+      <c r="E23">
+        <v>29</v>
+      </c>
+      <c r="F23">
+        <v>90460731000</v>
+      </c>
+      <c r="G23">
+        <v>542764386</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24">
+        <v>2025</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>27</v>
+      </c>
+      <c r="E24">
+        <v>27</v>
+      </c>
+      <c r="F24">
+        <v>92365037500</v>
+      </c>
+      <c r="G24">
+        <v>553716225</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25">
+        <v>2025</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>27</v>
+      </c>
+      <c r="E25">
+        <v>27</v>
+      </c>
+      <c r="F25">
+        <v>90556280789</v>
+      </c>
+      <c r="G25">
+        <v>543337685</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26">
+        <v>2025</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+      <c r="D26">
+        <v>27</v>
+      </c>
+      <c r="E26">
+        <v>27</v>
+      </c>
+      <c r="F26">
+        <v>94649760333.3333</v>
+      </c>
+      <c r="G26">
+        <v>567898562</v>
       </c>
     </row>
   </sheetData>
@@ -1741,17 +1820,13 @@
   <sheetPr/>
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="5"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="3" max="5" width="19.4545454545455" customWidth="1"/>
-    <col min="6" max="6" width="21.0909090909091" customWidth="1"/>
-    <col min="7" max="8" width="17.1818181818182"/>
-    <col min="9" max="10" width="18.3636363636364"/>
+    <col min="1" max="1" width="19.9090909090909" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1762,28 +1837,28 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1793,28 +1868,28 @@
       <c r="B2">
         <v>2025</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>36720000000</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2">
         <v>71660000000</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2">
         <v>121320000000</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2">
         <v>202200000000</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2">
         <v>1577200000</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2">
         <v>3154400000</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2">
         <v>5231600000</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2">
         <v>7886000000</v>
       </c>
     </row>
@@ -1825,28 +1900,28 @@
       <c r="B3">
         <v>2025</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>22065000000</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3">
         <v>132390000000</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3">
         <v>264780000000</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3">
         <v>441300000000</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3">
         <v>1556950000</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3">
         <v>6316800000</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3">
         <v>12633600000</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3">
         <v>21056000000</v>
       </c>
     </row>
@@ -1857,28 +1932,28 @@
       <c r="B4">
         <v>2025</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>25350000000</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4">
         <v>76050000000</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4">
         <v>101400000000</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4">
         <v>169000000000</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4">
         <v>1304400000</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4">
         <v>2934900000</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4">
         <v>3913200000</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4">
         <v>6522000000</v>
       </c>
     </row>
@@ -1889,60 +1964,60 @@
       <c r="B5">
         <v>2025</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>5800000000</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5">
         <v>17400000000</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5">
         <v>34800000000</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5">
         <v>58000000000</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5">
         <v>270500000</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5">
         <v>811500000</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5">
         <v>1623000000</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5">
         <v>2705000000</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>2025</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>214772000000</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6">
         <v>429544000000</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6">
         <v>859089000000</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6">
         <v>1073861000000</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6">
         <v>1067000000</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6">
         <v>2133000000</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6">
         <v>4266000000</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6">
         <v>5333000000</v>
       </c>
     </row>

</xml_diff>